<commit_message>
7 times write, 1 time commit
</commit_message>
<xml_diff>
--- a/diary.xlsx
+++ b/diary.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,10 +771,100 @@
           <t>послушай это</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>2025-10-19 12:27:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>539011121</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Anna_Safonova_life</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Анна</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>diary_entry</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Чувствую себя хорошо, но ещё есть тревога</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-10-19 12:34:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6479033897</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>zhuravlstrogo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>diary_entry</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Хочу умереть</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-10-19 12:51:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6893133357</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nadzh_k</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>diary_entry</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Хочу начать любить свою жизнь</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-10-19 15:19:09</t>
         </is>
       </c>
     </row>
@@ -789,7 +879,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -889,6 +979,36 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6479033897</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>zhuravlstrogo</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-10-19 12:51:36</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Суицидальные мысли</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>diary</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Хочу умереть</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>